<commit_message>
added Ayat of the Day serving via API call
</commit_message>
<xml_diff>
--- a/src/assets/daily_content/Roman Urdu Ayat and Hadith.xlsx
+++ b/src/assets/daily_content/Roman Urdu Ayat and Hadith.xlsx
@@ -3,19 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Hadith" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Ayat" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Ayat_API" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="99">
   <si>
     <t>timestamp</t>
   </si>
@@ -210,6 +210,108 @@
   </si>
   <si>
     <t xml:space="preserve">(ALLAH ki Perwi) Ay Paghambar jesa tum ko hukam hota hai (uss per) aur jo log tumharay sath tayib huwey hein qaim raho aur had se tajawuz na karna wo tumharay sab amal ko dekh raha hai. Soorah Hood 11. Ayat 112</t>
+  </si>
+  <si>
+    <t>Topic</t>
+  </si>
+  <si>
+    <t>Surah</t>
+  </si>
+  <si>
+    <t>Ayat</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Jannat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allah ki Azmat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aqal walon ke liye nishaniyah</t>
+  </si>
+  <si>
+    <t>Saabir</t>
+  </si>
+  <si>
+    <t>Shirk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allah ka waada</t>
+  </si>
+  <si>
+    <t>Rizq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allah ki naimatein</t>
+  </si>
+  <si>
+    <t>Nama-e-Amaal</t>
+  </si>
+  <si>
+    <t>Rah-e-Raast</t>
+  </si>
+  <si>
+    <t>Huqooq-ul-Ibad</t>
+  </si>
+  <si>
+    <t>Fasting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imaan waalon ki pehchan</t>
+  </si>
+  <si>
+    <t>Takkabur</t>
+  </si>
+  <si>
+    <t>Ayat-ul-Kursi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insan ki tang dili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Imaan aur Namaz</t>
+  </si>
+  <si>
+    <t>Qayamat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allah ka Kalaam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neyk Amaal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sab Jahanon Ka maalik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Raat aur Din</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bani Israel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Surah Yunus</t>
+  </si>
+  <si>
+    <t>Quran-e-Mufasil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dunya ki Khwahish</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazrat Nooh AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hazrat Shoaib AS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jhootay Mabood</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allah Ki perwi</t>
   </si>
 </sst>
 </file>
@@ -252,7 +354,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -276,6 +378,16 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="160" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -3891,6 +4003,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="17.421875"/>
+  </cols>
   <sheetData>
     <row r="1" ht="16.5">
       <c r="A1" s="1" t="s">
@@ -4814,7 +4929,7 @@
       <c r="A10" s="3">
         <v>45020</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="8" t="s">
         <v>42</v>
       </c>
       <c r="C10" s="1"/>
@@ -6038,7 +6153,7 @@
       <c r="A22" s="3">
         <v>45032</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="1"/>
@@ -6140,7 +6255,7 @@
       <c r="A23" s="3">
         <v>45033</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>55</v>
       </c>
       <c r="C23" s="1"/>
@@ -6242,7 +6357,7 @@
       <c r="A24" s="3">
         <v>45034</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="1"/>
@@ -6344,7 +6459,7 @@
       <c r="A25" s="3">
         <v>45035</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>57</v>
       </c>
       <c r="C25" s="1"/>
@@ -6446,7 +6561,7 @@
       <c r="A26" s="3">
         <v>45036</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>58</v>
       </c>
       <c r="C26" s="1"/>
@@ -6548,7 +6663,7 @@
       <c r="A27" s="3">
         <v>45037</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>59</v>
       </c>
     </row>
@@ -6556,7 +6671,7 @@
       <c r="A28" s="3">
         <v>45038</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>60</v>
       </c>
     </row>
@@ -6564,7 +6679,7 @@
       <c r="A29" s="3">
         <v>45039</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -6572,7 +6687,7 @@
       <c r="A30" s="3">
         <v>45040</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="9" t="s">
         <v>62</v>
       </c>
     </row>
@@ -6580,7 +6695,7 @@
       <c r="A31" s="3">
         <v>45041</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>63</v>
       </c>
     </row>
@@ -6609,7 +6724,587 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
-  <sheetData/>
+  <cols>
+    <col bestFit="1" min="1" max="1" width="17.421875"/>
+    <col bestFit="1" min="2" max="2" width="25.421875"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25">
+      <c r="A2" s="10">
+        <v>45012</v>
+      </c>
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" ht="14.25">
+      <c r="A3" s="10">
+        <v>45013</v>
+      </c>
+      <c r="B3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3">
+        <v>15</v>
+      </c>
+      <c r="D3">
+        <v>85</v>
+      </c>
+      <c r="E3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" ht="14.25">
+      <c r="A4" s="10">
+        <v>45014</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="A5" s="10">
+        <v>45015</v>
+      </c>
+      <c r="B5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5">
+        <v>16</v>
+      </c>
+      <c r="D5">
+        <v>41</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="A6" s="10">
+        <v>45016</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6">
+        <v>16</v>
+      </c>
+      <c r="D6">
+        <v>53</v>
+      </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="A7" s="10">
+        <v>45017</v>
+      </c>
+      <c r="B7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7">
+        <v>16</v>
+      </c>
+      <c r="D7">
+        <v>61</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" ht="14.25">
+      <c r="A8" s="10">
+        <v>45018</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8">
+        <v>16</v>
+      </c>
+      <c r="D8">
+        <v>71</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="A9" s="10">
+        <v>45019</v>
+      </c>
+      <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9">
+        <v>16</v>
+      </c>
+      <c r="D9">
+        <v>72</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="A10" s="10">
+        <v>45020</v>
+      </c>
+      <c r="B10" t="s">
+        <v>77</v>
+      </c>
+      <c r="C10">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>13</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="A11" s="10">
+        <v>45021</v>
+      </c>
+      <c r="B11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11">
+        <v>17</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="A12" s="10">
+        <v>45022</v>
+      </c>
+      <c r="B12" t="s">
+        <v>79</v>
+      </c>
+      <c r="C12">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>26</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="A13" s="10">
+        <v>45023</v>
+      </c>
+      <c r="B13" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>184</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="A14" s="10">
+        <v>45024</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>112</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" ht="14.25">
+      <c r="A15" s="10">
+        <v>45025</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15">
+        <v>17</v>
+      </c>
+      <c r="D15">
+        <v>36</v>
+      </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
+      <c r="F15" s="8"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="A16" s="10">
+        <v>45026</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>255</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="A17" s="10">
+        <v>45027</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17">
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <v>100</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="A18" s="10">
+        <v>45028</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>42</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18" s="7"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="A19" s="10">
+        <v>45029</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>47</v>
+      </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="A20" s="10">
+        <v>45030</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <v>105</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="A21" s="10">
+        <v>45031</v>
+      </c>
+      <c r="B21" t="s">
+        <v>87</v>
+      </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <v>106</v>
+      </c>
+      <c r="E21">
+        <v>2</v>
+      </c>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="A22" s="10">
+        <v>45032</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22">
+        <v>110</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22" s="9"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="A23" s="10">
+        <v>45033</v>
+      </c>
+      <c r="B23" t="s">
+        <v>89</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>115</v>
+      </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
+      <c r="F23" s="11"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="A24" s="10">
+        <v>45034</v>
+      </c>
+      <c r="B24" t="s">
+        <v>90</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>67</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24" s="9"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="A25" s="10">
+        <v>45035</v>
+      </c>
+      <c r="B25" t="s">
+        <v>91</v>
+      </c>
+      <c r="C25">
+        <v>10</v>
+      </c>
+      <c r="D25">
+        <v>93</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25" s="11"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="A26" s="10">
+        <v>45036</v>
+      </c>
+      <c r="B26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C26">
+        <v>10</v>
+      </c>
+      <c r="D26">
+        <v>99</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="A27" s="10">
+        <v>45037</v>
+      </c>
+      <c r="B27" t="s">
+        <v>93</v>
+      </c>
+      <c r="C27">
+        <v>11</v>
+      </c>
+      <c r="D27">
+        <v>12</v>
+      </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="A28" s="10">
+        <v>45038</v>
+      </c>
+      <c r="B28" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28">
+        <v>11</v>
+      </c>
+      <c r="D28">
+        <v>15</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" ht="14.25">
+      <c r="A29" s="10">
+        <v>45039</v>
+      </c>
+      <c r="B29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>36</v>
+      </c>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29" s="9"/>
+    </row>
+    <row r="30" ht="14.25">
+      <c r="A30" s="10">
+        <v>45040</v>
+      </c>
+      <c r="B30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>94</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30" s="9"/>
+    </row>
+    <row r="31" ht="14.25">
+      <c r="A31" s="10">
+        <v>45041</v>
+      </c>
+      <c r="B31" t="s">
+        <v>97</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>101</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" ht="14.25">
+      <c r="A32" s="10">
+        <v>45042</v>
+      </c>
+      <c r="B32" t="s">
+        <v>98</v>
+      </c>
+      <c r="C32">
+        <v>11</v>
+      </c>
+      <c r="D32">
+        <v>112</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+  </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>